<commit_message>
Improve 'config.json' to support both action types and add configuration validation
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myt\Desktop\Repositories\GithubTimeMachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC66EF92-A7C7-4352-BB39-F6EABB45B48C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BEA163-6B44-4218-8819-B70D85026EF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="815" xr2:uid="{217DBFA2-DA9B-4918-96B7-2C9E47E85EDD}"/>
   </bookViews>
@@ -667,7 +667,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -855,31 +857,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="10">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2" s="11">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G2" s="11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K2" s="11">
         <v>0</v>
@@ -897,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q2" s="11">
         <v>0</v>
@@ -906,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T2" s="11">
         <v>0</v>
@@ -978,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="AQ2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AR2" s="11">
         <v>0</v>
@@ -993,22 +995,22 @@
         <v>0</v>
       </c>
       <c r="AV2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW2" s="11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AX2" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY2" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA2" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB2" s="19">
         <v>0</v>
@@ -1019,163 +1021,163 @@
         <v>1</v>
       </c>
       <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>3</v>
+      </c>
+      <c r="D3" s="13">
+        <v>5</v>
+      </c>
+      <c r="E3" s="13">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>7</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="13">
+        <v>7</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="N3" s="13">
+        <v>0</v>
+      </c>
+      <c r="O3" s="13">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="13">
+        <v>0</v>
+      </c>
+      <c r="R3" s="13">
+        <v>0</v>
+      </c>
+      <c r="S3" s="13">
+        <v>7</v>
+      </c>
+      <c r="T3" s="13">
+        <v>0</v>
+      </c>
+      <c r="U3" s="13">
+        <v>0</v>
+      </c>
+      <c r="V3" s="13">
+        <v>0</v>
+      </c>
+      <c r="W3" s="13">
+        <v>0</v>
+      </c>
+      <c r="X3" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="13">
+        <v>7</v>
+      </c>
+      <c r="AR3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="13">
+        <v>7</v>
+      </c>
+      <c r="AW3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="13">
+        <v>7</v>
+      </c>
+      <c r="AY3" s="13">
+        <v>5</v>
+      </c>
+      <c r="AZ3" s="13">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB3" s="19">
         <v>-1</v>
-      </c>
-      <c r="C3" s="13">
-        <v>4</v>
-      </c>
-      <c r="D3" s="13">
-        <v>3</v>
-      </c>
-      <c r="E3" s="13">
-        <v>2</v>
-      </c>
-      <c r="F3" s="13">
-        <v>1</v>
-      </c>
-      <c r="G3" s="13">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13">
-        <v>0</v>
-      </c>
-      <c r="J3" s="13">
-        <v>1</v>
-      </c>
-      <c r="K3" s="13">
-        <v>1</v>
-      </c>
-      <c r="L3" s="13">
-        <v>0</v>
-      </c>
-      <c r="M3" s="13">
-        <v>0</v>
-      </c>
-      <c r="N3" s="13">
-        <v>0</v>
-      </c>
-      <c r="O3" s="13">
-        <v>0</v>
-      </c>
-      <c r="P3" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="13">
-        <v>0</v>
-      </c>
-      <c r="R3" s="13">
-        <v>0</v>
-      </c>
-      <c r="S3" s="13">
-        <v>0</v>
-      </c>
-      <c r="T3" s="13">
-        <v>0</v>
-      </c>
-      <c r="U3" s="13">
-        <v>0</v>
-      </c>
-      <c r="V3" s="13">
-        <v>0</v>
-      </c>
-      <c r="W3" s="13">
-        <v>10</v>
-      </c>
-      <c r="X3" s="13">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="13">
-        <v>10</v>
-      </c>
-      <c r="Z3" s="13">
-        <v>10</v>
-      </c>
-      <c r="AA3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="13">
-        <v>10</v>
-      </c>
-      <c r="AE3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="13">
-        <v>10</v>
-      </c>
-      <c r="AH3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="13">
-        <v>0</v>
-      </c>
-      <c r="BA3" s="17">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="19">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -1183,163 +1185,163 @@
         <v>2</v>
       </c>
       <c r="B4" s="12">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13">
+        <v>5</v>
+      </c>
+      <c r="D4" s="13">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>5</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
+        <v>5</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>5</v>
+      </c>
+      <c r="M4" s="13">
+        <v>5</v>
+      </c>
+      <c r="N4" s="13">
+        <v>5</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>0</v>
+      </c>
+      <c r="R4" s="13">
+        <v>0</v>
+      </c>
+      <c r="S4" s="13">
+        <v>5</v>
+      </c>
+      <c r="T4" s="13">
+        <v>0</v>
+      </c>
+      <c r="U4" s="13">
+        <v>0</v>
+      </c>
+      <c r="V4" s="13">
+        <v>5</v>
+      </c>
+      <c r="W4" s="13">
+        <v>5</v>
+      </c>
+      <c r="X4" s="13">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AJ4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AK4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AL4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AN4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AO4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AP4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AR4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="13">
+        <v>3</v>
+      </c>
+      <c r="AW4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AZ4" s="13">
+        <v>4</v>
+      </c>
+      <c r="BA4" s="17">
+        <v>3</v>
+      </c>
+      <c r="BB4" s="19">
         <v>-1</v>
-      </c>
-      <c r="C4" s="13">
-        <v>3</v>
-      </c>
-      <c r="D4" s="13">
-        <v>2</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0</v>
-      </c>
-      <c r="J4" s="13">
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13">
-        <v>1</v>
-      </c>
-      <c r="N4" s="13">
-        <v>3</v>
-      </c>
-      <c r="O4" s="13">
-        <v>5</v>
-      </c>
-      <c r="P4" s="13">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>0</v>
-      </c>
-      <c r="R4" s="13">
-        <v>0</v>
-      </c>
-      <c r="S4" s="13">
-        <v>0</v>
-      </c>
-      <c r="T4" s="13">
-        <v>0</v>
-      </c>
-      <c r="U4" s="13">
-        <v>0</v>
-      </c>
-      <c r="V4" s="13">
-        <v>10</v>
-      </c>
-      <c r="W4" s="13">
-        <v>0</v>
-      </c>
-      <c r="X4" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AD4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AE4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AF4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AG4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AH4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AI4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="13">
-        <v>3</v>
-      </c>
-      <c r="AO4" s="13">
-        <v>5</v>
-      </c>
-      <c r="AP4" s="13">
-        <v>3</v>
-      </c>
-      <c r="AQ4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AY4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="13">
-        <v>1</v>
-      </c>
-      <c r="BA4" s="17">
-        <v>1</v>
-      </c>
-      <c r="BB4" s="19">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
@@ -1347,163 +1349,163 @@
         <v>3</v>
       </c>
       <c r="B5" s="12">
+        <v>5</v>
+      </c>
+      <c r="C5" s="13">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13">
+        <v>3</v>
+      </c>
+      <c r="I5" s="13">
+        <v>3</v>
+      </c>
+      <c r="J5" s="13">
+        <v>3</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <v>3</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
+        <v>3</v>
+      </c>
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>0</v>
+      </c>
+      <c r="R5" s="13">
+        <v>0</v>
+      </c>
+      <c r="S5" s="13">
+        <v>3</v>
+      </c>
+      <c r="T5" s="13">
+        <v>0</v>
+      </c>
+      <c r="U5" s="13">
+        <v>0</v>
+      </c>
+      <c r="V5" s="13">
+        <v>3</v>
+      </c>
+      <c r="W5" s="13">
+        <v>0</v>
+      </c>
+      <c r="X5" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AJ5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AL5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AN5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AR5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AU5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AV5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AW5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="13">
+        <v>5</v>
+      </c>
+      <c r="BA5" s="17">
+        <v>1</v>
+      </c>
+      <c r="BB5" s="19">
         <v>-1</v>
-      </c>
-      <c r="C5" s="13">
-        <v>2</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13">
-        <v>0</v>
-      </c>
-      <c r="J5" s="13">
-        <v>0</v>
-      </c>
-      <c r="K5" s="13">
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
-        <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>5</v>
-      </c>
-      <c r="O5" s="13">
-        <v>10</v>
-      </c>
-      <c r="P5" s="13">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>0</v>
-      </c>
-      <c r="R5" s="13">
-        <v>0</v>
-      </c>
-      <c r="S5" s="13">
-        <v>0</v>
-      </c>
-      <c r="T5" s="13">
-        <v>0</v>
-      </c>
-      <c r="U5" s="13">
-        <v>1</v>
-      </c>
-      <c r="V5" s="13">
-        <v>10</v>
-      </c>
-      <c r="W5" s="13">
-        <v>0</v>
-      </c>
-      <c r="X5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="13">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="13">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="13">
-        <v>10</v>
-      </c>
-      <c r="AE5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="13">
-        <v>10</v>
-      </c>
-      <c r="AH5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="13">
-        <v>5</v>
-      </c>
-      <c r="AO5" s="13">
-        <v>10</v>
-      </c>
-      <c r="AP5" s="13">
-        <v>5</v>
-      </c>
-      <c r="AQ5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="13">
-        <v>1</v>
-      </c>
-      <c r="AZ5" s="13">
-        <v>1</v>
-      </c>
-      <c r="BA5" s="17">
-        <v>2</v>
-      </c>
-      <c r="BB5" s="19">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
@@ -1511,163 +1513,163 @@
         <v>4</v>
       </c>
       <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13">
+        <v>7</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>5</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>5</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13">
+        <v>5</v>
+      </c>
+      <c r="M6" s="13">
+        <v>5</v>
+      </c>
+      <c r="N6" s="13">
+        <v>5</v>
+      </c>
+      <c r="O6" s="13">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>0</v>
+      </c>
+      <c r="R6" s="13">
+        <v>0</v>
+      </c>
+      <c r="S6" s="13">
+        <v>5</v>
+      </c>
+      <c r="T6" s="13">
+        <v>0</v>
+      </c>
+      <c r="U6" s="13">
+        <v>0</v>
+      </c>
+      <c r="V6" s="13">
+        <v>5</v>
+      </c>
+      <c r="W6" s="13">
+        <v>0</v>
+      </c>
+      <c r="X6" s="13">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AJ6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AR6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AU6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="13">
+        <v>5</v>
+      </c>
+      <c r="AW6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="13">
+        <v>1</v>
+      </c>
+      <c r="AZ6" s="13">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="19">
         <v>-1</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
-      <c r="F6" s="13">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
-      <c r="I6" s="13">
-        <v>0</v>
-      </c>
-      <c r="J6" s="13">
-        <v>0</v>
-      </c>
-      <c r="K6" s="13">
-        <v>0</v>
-      </c>
-      <c r="L6" s="13">
-        <v>0</v>
-      </c>
-      <c r="M6" s="13">
-        <v>0</v>
-      </c>
-      <c r="N6" s="13">
-        <v>3</v>
-      </c>
-      <c r="O6" s="13">
-        <v>5</v>
-      </c>
-      <c r="P6" s="13">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="13">
-        <v>0</v>
-      </c>
-      <c r="R6" s="13">
-        <v>0</v>
-      </c>
-      <c r="S6" s="13">
-        <v>0</v>
-      </c>
-      <c r="T6" s="13">
-        <v>0</v>
-      </c>
-      <c r="U6" s="13">
-        <v>1</v>
-      </c>
-      <c r="V6" s="13">
-        <v>10</v>
-      </c>
-      <c r="W6" s="13">
-        <v>0</v>
-      </c>
-      <c r="X6" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="13">
-        <v>10</v>
-      </c>
-      <c r="AD6" s="13">
-        <v>10</v>
-      </c>
-      <c r="AE6" s="13">
-        <v>10</v>
-      </c>
-      <c r="AF6" s="13">
-        <v>10</v>
-      </c>
-      <c r="AG6" s="13">
-        <v>10</v>
-      </c>
-      <c r="AH6" s="13">
-        <v>10</v>
-      </c>
-      <c r="AI6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="13">
-        <v>3</v>
-      </c>
-      <c r="AO6" s="13">
-        <v>5</v>
-      </c>
-      <c r="AP6" s="13">
-        <v>3</v>
-      </c>
-      <c r="AQ6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AR6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AY6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AZ6" s="13">
-        <v>2</v>
-      </c>
-      <c r="BA6" s="17">
-        <v>3</v>
-      </c>
-      <c r="BB6" s="19">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
@@ -1678,19 +1680,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F7" s="13">
         <v>0</v>
       </c>
       <c r="G7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7" s="13">
         <v>0</v>
@@ -1699,13 +1701,13 @@
         <v>0</v>
       </c>
       <c r="J7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K7" s="13">
         <v>0</v>
       </c>
       <c r="L7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M7" s="13">
         <v>0</v>
@@ -1717,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="13">
         <v>0</v>
@@ -1726,67 +1728,67 @@
         <v>0</v>
       </c>
       <c r="S7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T7" s="13">
         <v>0</v>
       </c>
       <c r="U7" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V7" s="13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="W7" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X7" s="13">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Y7" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="13">
         <v>0</v>
       </c>
       <c r="AB7" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AD7" s="13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AF7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="13">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AH7" s="13">
         <v>0</v>
       </c>
       <c r="AI7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AJ7" s="13">
         <v>0</v>
       </c>
       <c r="AK7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AL7" s="13">
         <v>0</v>
       </c>
       <c r="AM7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AN7" s="13">
         <v>0</v>
@@ -1798,40 +1800,40 @@
         <v>0</v>
       </c>
       <c r="AQ7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AR7" s="13">
         <v>0</v>
       </c>
       <c r="AS7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AU7" s="13">
         <v>0</v>
       </c>
       <c r="AV7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AW7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX7" s="13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AY7" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AZ7" s="13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA7" s="17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BB7" s="19">
-        <v>5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1845,16 +1847,16 @@
         <v>1</v>
       </c>
       <c r="D8" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H8" s="15">
         <v>0</v>
@@ -1863,52 +1865,52 @@
         <v>0</v>
       </c>
       <c r="J8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K8" s="15">
         <v>0</v>
       </c>
       <c r="L8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O8" s="15">
         <v>0</v>
       </c>
       <c r="P8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R8" s="15">
         <v>0</v>
       </c>
       <c r="S8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U8" s="15">
         <v>0</v>
       </c>
       <c r="V8" s="15">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="W8" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="X8" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Y8" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="15">
         <v>0</v>
@@ -1920,16 +1922,16 @@
         <v>0</v>
       </c>
       <c r="AC8" s="15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE8" s="15">
         <v>0</v>
       </c>
       <c r="AF8" s="15">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AG8" s="15">
         <v>0</v>
@@ -1938,19 +1940,19 @@
         <v>0</v>
       </c>
       <c r="AI8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AJ8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL8" s="15">
         <v>0</v>
       </c>
       <c r="AM8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AN8" s="15">
         <v>0</v>
@@ -1962,40 +1964,40 @@
         <v>0</v>
       </c>
       <c r="AQ8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AR8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AS8" s="15">
         <v>0</v>
       </c>
       <c r="AT8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AU8" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AV8" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AW8" s="15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AX8" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AY8" s="15">
         <v>3</v>
       </c>
       <c r="AZ8" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="BA8" s="18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BB8" s="20">
-        <v>6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -8266,10 +8268,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B95B46F-0358-4049-BFC9-6098CCE66252}">
   <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:BB9"/>
+  <dimension ref="A1:BB11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+      <selection activeCell="BB8" sqref="B2:BB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8282,7 +8284,9 @@
     <col min="7" max="7" width="2.7109375" customWidth="1"/>
     <col min="8" max="9" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="25" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="25" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" bestFit="1" customWidth="1"/>
     <col min="27" max="37" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="3" bestFit="1" customWidth="1"/>
@@ -8461,19 +8465,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2" s="11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H2" s="11">
         <v>0</v>
@@ -8482,7 +8486,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K2" s="11">
         <v>0</v>
@@ -8500,7 +8504,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q2" s="11">
         <v>0</v>
@@ -8509,7 +8513,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T2" s="11">
         <v>0</v>
@@ -8581,7 +8585,7 @@
         <v>0</v>
       </c>
       <c r="AQ2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AR2" s="11">
         <v>0</v>
@@ -8596,19 +8600,19 @@
         <v>0</v>
       </c>
       <c r="AV2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW2" s="11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AX2" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY2" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA2" s="17">
         <v>0</v>
@@ -8622,22 +8626,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F3" s="13">
         <v>0</v>
       </c>
       <c r="G3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H3" s="13">
         <v>0</v>
@@ -8646,7 +8650,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K3" s="13">
         <v>0</v>
@@ -8664,7 +8668,7 @@
         <v>0</v>
       </c>
       <c r="P3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="13">
         <v>0</v>
@@ -8673,7 +8677,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T3" s="13">
         <v>0</v>
@@ -8745,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="AQ3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AR3" s="13">
         <v>0</v>
@@ -8760,22 +8764,22 @@
         <v>0</v>
       </c>
       <c r="AV3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AW3" s="13">
         <v>0</v>
       </c>
       <c r="AX3" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AY3" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA3" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB3" s="19">
         <v>-1</v>
@@ -8786,13 +8790,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
@@ -8801,7 +8805,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4" s="13">
         <v>0</v>
@@ -8810,25 +8814,25 @@
         <v>0</v>
       </c>
       <c r="J4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K4" s="13">
         <v>0</v>
       </c>
       <c r="L4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O4" s="13">
         <v>0</v>
       </c>
       <c r="P4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q4" s="13">
         <v>0</v>
@@ -8837,7 +8841,7 @@
         <v>0</v>
       </c>
       <c r="S4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T4" s="13">
         <v>0</v>
@@ -8846,13 +8850,13 @@
         <v>0</v>
       </c>
       <c r="V4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="13">
         <v>0</v>
@@ -8867,49 +8871,49 @@
         <v>0</v>
       </c>
       <c r="AC4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD4" s="13">
         <v>0</v>
       </c>
       <c r="AE4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF4" s="13">
         <v>0</v>
       </c>
       <c r="AG4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH4" s="13">
         <v>0</v>
       </c>
       <c r="AI4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL4" s="13">
         <v>0</v>
       </c>
       <c r="AM4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP4" s="13">
         <v>0</v>
       </c>
       <c r="AQ4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR4" s="13">
         <v>0</v>
@@ -8924,7 +8928,7 @@
         <v>0</v>
       </c>
       <c r="AV4" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW4" s="13">
         <v>0</v>
@@ -8933,13 +8937,13 @@
         <v>0</v>
       </c>
       <c r="AY4" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ4" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA4" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB4" s="19">
         <v>-1</v>
@@ -8950,10 +8954,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D5" s="13">
         <v>0</v>
@@ -8965,34 +8969,34 @@
         <v>0</v>
       </c>
       <c r="G5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="13">
         <v>0</v>
       </c>
       <c r="L5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M5" s="13">
         <v>0</v>
       </c>
       <c r="N5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O5" s="13">
         <v>0</v>
       </c>
       <c r="P5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="13">
         <v>0</v>
@@ -9001,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T5" s="13">
         <v>0</v>
@@ -9010,13 +9014,13 @@
         <v>0</v>
       </c>
       <c r="V5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W5" s="13">
         <v>0</v>
       </c>
       <c r="X5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y5" s="13">
         <v>0</v>
@@ -9031,37 +9035,37 @@
         <v>0</v>
       </c>
       <c r="AC5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD5" s="13">
         <v>0</v>
       </c>
       <c r="AE5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF5" s="13">
         <v>0</v>
       </c>
       <c r="AG5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH5" s="13">
         <v>0</v>
       </c>
       <c r="AI5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ5" s="13">
         <v>0</v>
       </c>
       <c r="AK5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL5" s="13">
         <v>0</v>
       </c>
       <c r="AM5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN5" s="13">
         <v>0</v>
@@ -9073,7 +9077,7 @@
         <v>0</v>
       </c>
       <c r="AQ5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR5" s="13">
         <v>0</v>
@@ -9082,13 +9086,13 @@
         <v>0</v>
       </c>
       <c r="AT5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AU5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AV5" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW5" s="13">
         <v>0</v>
@@ -9100,10 +9104,10 @@
         <v>0</v>
       </c>
       <c r="AZ5" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA5" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB5" s="19">
         <v>-1</v>
@@ -9114,13 +9118,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E6" s="13">
         <v>0</v>
@@ -9129,7 +9133,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H6" s="13">
         <v>0</v>
@@ -9138,25 +9142,25 @@
         <v>0</v>
       </c>
       <c r="J6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6" s="13">
         <v>0</v>
       </c>
       <c r="L6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O6" s="13">
         <v>0</v>
       </c>
       <c r="P6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="13">
         <v>0</v>
@@ -9165,7 +9169,7 @@
         <v>0</v>
       </c>
       <c r="S6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T6" s="13">
         <v>0</v>
@@ -9174,13 +9178,13 @@
         <v>0</v>
       </c>
       <c r="V6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W6" s="13">
         <v>0</v>
       </c>
       <c r="X6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y6" s="13">
         <v>0</v>
@@ -9195,37 +9199,37 @@
         <v>0</v>
       </c>
       <c r="AC6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD6" s="13">
         <v>0</v>
       </c>
       <c r="AE6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF6" s="13">
         <v>0</v>
       </c>
       <c r="AG6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH6" s="13">
         <v>0</v>
       </c>
       <c r="AI6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ6" s="13">
         <v>0</v>
       </c>
       <c r="AK6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL6" s="13">
         <v>0</v>
       </c>
       <c r="AM6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN6" s="13">
         <v>0</v>
@@ -9237,7 +9241,7 @@
         <v>0</v>
       </c>
       <c r="AQ6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR6" s="13">
         <v>0</v>
@@ -9246,13 +9250,13 @@
         <v>0</v>
       </c>
       <c r="AT6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU6" s="13">
         <v>0</v>
       </c>
       <c r="AV6" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW6" s="13">
         <v>0</v>
@@ -9261,10 +9265,10 @@
         <v>0</v>
       </c>
       <c r="AY6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA6" s="17">
         <v>0</v>
@@ -9278,22 +9282,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F7" s="13">
         <v>0</v>
       </c>
       <c r="G7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7" s="13">
         <v>0</v>
@@ -9302,13 +9306,13 @@
         <v>0</v>
       </c>
       <c r="J7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K7" s="13">
         <v>0</v>
       </c>
       <c r="L7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M7" s="13">
         <v>0</v>
@@ -9320,7 +9324,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="13">
         <v>0</v>
@@ -9329,7 +9333,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T7" s="13">
         <v>0</v>
@@ -9338,13 +9342,13 @@
         <v>0</v>
       </c>
       <c r="V7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="W7" s="13">
         <v>0</v>
       </c>
       <c r="X7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y7" s="13">
         <v>0</v>
@@ -9359,37 +9363,37 @@
         <v>0</v>
       </c>
       <c r="AC7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AD7" s="13">
         <v>0</v>
       </c>
       <c r="AE7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AF7" s="13">
         <v>0</v>
       </c>
       <c r="AG7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH7" s="13">
         <v>0</v>
       </c>
       <c r="AI7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AJ7" s="13">
         <v>0</v>
       </c>
       <c r="AK7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AL7" s="13">
         <v>0</v>
       </c>
       <c r="AM7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AN7" s="13">
         <v>0</v>
@@ -9401,7 +9405,7 @@
         <v>0</v>
       </c>
       <c r="AQ7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AR7" s="13">
         <v>0</v>
@@ -9410,22 +9414,22 @@
         <v>0</v>
       </c>
       <c r="AT7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AU7" s="13">
         <v>0</v>
       </c>
       <c r="AV7" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AW7" s="13">
         <v>0</v>
       </c>
       <c r="AX7" s="13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AY7" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ7" s="13">
         <v>0</v>
@@ -9445,19 +9449,19 @@
         <v>0</v>
       </c>
       <c r="C8" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H8" s="15">
         <v>0</v>
@@ -9466,49 +9470,49 @@
         <v>0</v>
       </c>
       <c r="J8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K8" s="15">
         <v>0</v>
       </c>
       <c r="L8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O8" s="15">
         <v>0</v>
       </c>
       <c r="P8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R8" s="15">
         <v>0</v>
       </c>
       <c r="S8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U8" s="15">
         <v>0</v>
       </c>
       <c r="V8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="X8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Y8" s="15">
         <v>0</v>
@@ -9526,13 +9530,13 @@
         <v>0</v>
       </c>
       <c r="AD8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE8" s="15">
         <v>0</v>
       </c>
       <c r="AF8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AG8" s="15">
         <v>0</v>
@@ -9541,19 +9545,19 @@
         <v>0</v>
       </c>
       <c r="AI8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AJ8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL8" s="15">
         <v>0</v>
       </c>
       <c r="AM8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AN8" s="15">
         <v>0</v>
@@ -9565,34 +9569,34 @@
         <v>0</v>
       </c>
       <c r="AQ8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AR8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AS8" s="15">
         <v>0</v>
       </c>
       <c r="AT8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AU8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AV8" s="15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW8" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AX8" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY8" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ8" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA8" s="18">
         <v>0</v>
@@ -9763,8 +9767,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AW10" s="17"/>
+      <c r="AX10" s="17"/>
+      <c r="AY10" s="17"/>
+      <c r="AZ10" s="17"/>
+      <c r="BA10" s="17"/>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AX11" s="17"/>
+      <c r="AY11" s="17"/>
+      <c r="AZ11" s="17"/>
+      <c r="BA11" s="17"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:BB8">
+  <conditionalFormatting sqref="B2:BB8 AX11:BA11 AW10:BA10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -14341,7 +14358,7 @@
   <dimension ref="A1:BB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="BB8" sqref="B2:BB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14703,16 +14720,16 @@
         <v>0</v>
       </c>
       <c r="E3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="13">
         <v>0</v>
       </c>
       <c r="H3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="13">
         <v>0</v>
@@ -14730,7 +14747,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O3" s="13">
         <v>0</v>
@@ -14766,13 +14783,13 @@
         <v>0</v>
       </c>
       <c r="Z3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3" s="13">
         <v>0</v>
@@ -14784,10 +14801,10 @@
         <v>0</v>
       </c>
       <c r="AF3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH3" s="13">
         <v>0</v>
@@ -14799,7 +14816,7 @@
         <v>0</v>
       </c>
       <c r="AK3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL3" s="13">
         <v>0</v>
@@ -14808,7 +14825,7 @@
         <v>0</v>
       </c>
       <c r="AN3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO3" s="13">
         <v>0</v>
@@ -14823,7 +14840,7 @@
         <v>0</v>
       </c>
       <c r="AS3" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT3" s="13">
         <v>0</v>
@@ -14861,22 +14878,22 @@
         <v>-1</v>
       </c>
       <c r="C4" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
       </c>
       <c r="F4" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="13">
         <v>0</v>
       </c>
       <c r="H4" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="13">
         <v>0</v>
@@ -14894,7 +14911,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4" s="13">
         <v>0</v>
@@ -14930,10 +14947,10 @@
         <v>0</v>
       </c>
       <c r="Z4" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB4" s="13">
         <v>0</v>
@@ -14951,7 +14968,7 @@
         <v>0</v>
       </c>
       <c r="AG4" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH4" s="13">
         <v>0</v>
@@ -14972,7 +14989,7 @@
         <v>0</v>
       </c>
       <c r="AN4" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO4" s="13">
         <v>0</v>
@@ -14987,7 +15004,7 @@
         <v>0</v>
       </c>
       <c r="AS4" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT4" s="13">
         <v>0</v>
@@ -15025,160 +15042,160 @@
         <v>-1</v>
       </c>
       <c r="C5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="13">
         <v>0</v>
       </c>
       <c r="M5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P5" s="13">
         <v>0</v>
       </c>
       <c r="Q5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="13">
         <v>0</v>
       </c>
       <c r="AA5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA5" s="17">
         <v>0</v>
       </c>
       <c r="BB5" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
@@ -15192,157 +15209,157 @@
         <v>0</v>
       </c>
       <c r="D6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="13">
         <v>0</v>
       </c>
       <c r="H6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="13">
         <v>0</v>
       </c>
       <c r="J6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="13">
         <v>0</v>
       </c>
       <c r="M6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6" s="13">
         <v>0</v>
       </c>
       <c r="Q6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R6" s="13">
         <v>0</v>
       </c>
       <c r="S6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" s="13">
         <v>0</v>
       </c>
       <c r="U6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH6" s="13">
         <v>0</v>
       </c>
       <c r="AI6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6" s="13">
         <v>0</v>
       </c>
       <c r="AK6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO6" s="13">
         <v>0</v>
       </c>
       <c r="AP6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="13">
         <v>0</v>
       </c>
       <c r="AR6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT6" s="13">
         <v>0</v>
       </c>
       <c r="AU6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV6" s="13">
         <v>0</v>
       </c>
       <c r="AW6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX6" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY6" s="13">
         <v>0</v>
       </c>
       <c r="AZ6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA6" s="17">
         <v>0</v>
       </c>
       <c r="BB6" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
@@ -15353,160 +15370,160 @@
         <v>0</v>
       </c>
       <c r="C7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7" s="13">
         <v>0</v>
       </c>
       <c r="J7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W7" s="13">
         <v>0</v>
       </c>
       <c r="X7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD7" s="13">
         <v>0</v>
       </c>
       <c r="AE7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7" s="13">
         <v>0</v>
       </c>
       <c r="AK7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM7" s="13">
         <v>0</v>
       </c>
       <c r="AN7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR7" s="13">
         <v>0</v>
       </c>
       <c r="AS7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW7" s="13">
         <v>0</v>
       </c>
       <c r="AX7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY7" s="13">
         <v>0</v>
       </c>
       <c r="AZ7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA7" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB7" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>